<commit_message>
add background change in side nav
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>事项</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -41,6 +41,10 @@
   </si>
   <si>
     <t>本地缓存localstorage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路由为空时回home.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -399,7 +403,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -452,8 +456,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>42790</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2"/>
     </row>

</xml_diff>

<commit_message>
add keydown and loading animation in login window
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>事项</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,6 +45,30 @@
   </si>
   <si>
     <t>路由为空时回home.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录界面错误提示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主界面提示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拖动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录时的keydown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录页面加载动画</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动登录</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -88,13 +112,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,17 +427,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -462,21 +489,80 @@
       <c r="B4" s="2">
         <v>42790</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
-    </row>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>42790</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>42790</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>42791</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42790</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>42790</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3">
+        <v>42791</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>42791</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3">
+        <v>42791</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>42791</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3">
+        <v>42791</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modify style of scroll bar and drag-region
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>事项</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,6 +73,10 @@
   </si>
   <si>
     <t>各个页面局部刷新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>滚动条样式</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -431,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -529,6 +533,12 @@
       <c r="B7" s="2">
         <v>42790</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>42791</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
@@ -583,6 +593,20 @@
         <v>5</v>
       </c>
       <c r="D11" s="2">
+        <v>42791</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3">
+        <v>42791</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
         <v>42791</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lecture notice and search in library part
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>事项</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -77,6 +77,34 @@
   </si>
   <si>
     <t>滚动条样式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动登录显示 cardnum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>局部刷新按钮禁止</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校园网已用流量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人文讲座预告</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改密码情况</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图书查询</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -435,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -448,7 +476,7 @@
     <col min="4" max="4" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,8 +489,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -476,7 +507,7 @@
         <v>42790</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -490,7 +521,7 @@
         <v>42790</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -504,7 +535,7 @@
         <v>42790</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -518,7 +549,7 @@
         <v>42791</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -526,7 +557,7 @@
         <v>42790</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -540,7 +571,7 @@
         <v>42791</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -554,7 +585,7 @@
         <v>42791</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -568,7 +599,7 @@
         <v>42791</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -582,7 +613,7 @@
         <v>42791</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -596,7 +627,7 @@
         <v>42791</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -608,6 +639,63 @@
       </c>
       <c r="D12" s="2">
         <v>42791</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3">
+        <v>42792</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3">
+        <v>42792</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="3">
+        <v>42792</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3">
+        <v>42792</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="3">
+        <v>42792</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="3">
+        <v>42792</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3">
+        <v>42792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some images and todo item
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>事项</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -105,6 +105,30 @@
   </si>
   <si>
     <t>图书查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教务处信息点击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主页重新排版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>×</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>找不到合适的处理逻辑过程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小化按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应用图标背景透明</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -148,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,6 +182,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -474,6 +501,7 @@
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.875" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -645,57 +673,126 @@
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3">
-        <v>42792</v>
-      </c>
+      <c r="B13" s="2">
+        <v>42792</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>42792</v>
+      </c>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="3">
-        <v>42792</v>
-      </c>
+      <c r="B14" s="2">
+        <v>42792</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="3">
-        <v>42792</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="2">
+        <v>42792</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>42792</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="3">
-        <v>42792</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D16" s="2">
+        <v>42792</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B17" s="2">
+        <v>42791</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>42792</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="3">
-        <v>42792</v>
+      <c r="D18" s="2">
+        <v>42792</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="2">
+        <v>42792</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>42793</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
+        <v>42792</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2">
+        <v>42792</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified the logic of refresh
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>事项</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,6 +129,26 @@
   </si>
   <si>
     <t>应用图标背景透明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更改刷新逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有必要性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>找不到合适的界面设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>版本信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -490,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -691,9 +711,13 @@
       <c r="B14" s="2">
         <v>42792</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
@@ -776,7 +800,9 @@
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="4"/>
+      <c r="D20" s="2">
+        <v>42793</v>
+      </c>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -786,13 +812,42 @@
       <c r="B21" s="2">
         <v>42792</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="B22" s="2">
+        <v>42803</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>42804</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="2">
+        <v>42805</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="2">
+        <v>42805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug of mdToast
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>事项</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -604,6 +604,12 @@
       <c r="B6" s="2">
         <v>42790</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>42806</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
@@ -812,7 +818,7 @@
       <c r="B21" s="2">
         <v>42792</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="4"/>
@@ -841,6 +847,12 @@
       <c r="B23" s="2">
         <v>42805</v>
       </c>
+      <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>42805</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
@@ -849,6 +861,8 @@
       <c r="B24" s="2">
         <v>42805</v>
       </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
modified width of md-list-item-text
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>事项</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -149,6 +149,10 @@
   </si>
   <si>
     <t>版本信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轮播图</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -510,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -864,6 +868,14 @@
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
     </row>
+    <row r="25" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="2">
+        <v>42806</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added version and modified user-agent
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>事项</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -517,7 +517,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -865,8 +865,12 @@
       <c r="B24" s="2">
         <v>42805</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
+      <c r="C24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>42809</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">

</xml_diff>